<commit_message>
feat: Add/update COVIDVAC for DHIS2v 2.30, 2.33
</commit_message>
<xml_diff>
--- a/metadata/COVIDVAC/COVIDVAC_COMPLETE_V1_DHIS2.30/reference.xlsx
+++ b/metadata/COVIDVAC/COVIDVAC_COMPLETE_V1_DHIS2.30/reference.xlsx
@@ -495,7 +495,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-04-23T07:49</v>
+        <v>2021-04-26T16:17</v>
       </c>
     </row>
     <row r="7">
@@ -503,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVIDVAC_COMPLETE_V1.2_DHIS2.30_2021-04-23T07:49</v>
+        <v>COVIDVAC_COMPLETE_V1.2_DHIS2.30_2021-04-26T16:17</v>
       </c>
     </row>
   </sheetData>
@@ -560,7 +560,7 @@
         <v>Johnson&amp;Johnson</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>cC2s7FgU4Us</v>
@@ -571,7 +571,7 @@
         <v>AstraZeneca/AZD12222</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>EkftcXiUiZZ</v>
@@ -626,7 +626,7 @@
         <v>Adult</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>Jkv8y0bywtg</v>
@@ -637,7 +637,7 @@
         <v>AstraZeneca/AZ-SKBio</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C11" s="5" t="str">
         <v>JpgLEcK4nl2</v>
@@ -659,7 +659,7 @@
         <v>Sinopharm/Coronavac</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C13" s="5" t="str">
         <v>lMNq0wL4MqR</v>
@@ -681,7 +681,7 @@
         <v>Pfizer/Biontech/Comirnaty</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C15" s="5" t="str">
         <v>lSQF5dQxJVP</v>
@@ -725,7 +725,7 @@
         <v>Moderna/mRNA-1273</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C19" s="5" t="str">
         <v>NEdeswIUJ7T</v>
@@ -736,7 +736,7 @@
         <v>Gamaleya/Sputnik V</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C20" s="4" t="str">
         <v>oi7CVBHqMIk</v>
@@ -747,7 +747,7 @@
         <v>Underlying conditions</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C21" s="5" t="str">
         <v>OKMPkKma5Ja</v>
@@ -791,7 +791,7 @@
         <v>Older adult</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C25" s="5" t="str">
         <v>T8aNcbtPKBo</v>
@@ -862,7 +862,7 @@
         <v>Older adult, Male</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>bgOEJC1SROA</v>
@@ -873,7 +873,7 @@
         <v>Pfizer/Biontech/Comirnaty</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2021-03-24</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>BurSMGyPjBI</v>
@@ -884,7 +884,7 @@
         <v>Moderna/mRNA-1273</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>c5WkU6fYL40</v>
@@ -906,7 +906,7 @@
         <v>Adult, Male, Underlying conditions</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>EEgOAHnVBPh</v>
@@ -928,7 +928,7 @@
         <v>Adult, Female</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C9" s="5" t="str">
         <v>G5DTdXwMaia</v>
@@ -939,7 +939,7 @@
         <v>Adult, Female, No underlying conditions</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>gSBt0sW2xt7</v>
@@ -950,7 +950,7 @@
         <v>Older adult, Male, Underlying conditions</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C11" s="5" t="str">
         <v>h36QRTxHjMG</v>
@@ -961,7 +961,7 @@
         <v>AstraZeneca/AZ-SKBio</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C12" s="4" t="str">
         <v>H4eiCaIeZQR</v>
@@ -972,7 +972,7 @@
         <v>Vaccine3</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C13" s="5" t="str">
         <v>HDF0FxE00WL</v>
@@ -983,7 +983,7 @@
         <v>Adult, Male, No underlying conditions</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C14" s="4" t="str">
         <v>Hgeo6ZzEURv</v>
@@ -1016,7 +1016,7 @@
         <v>Johnson&amp;Johnson</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C17" s="5" t="str">
         <v>j07LjUKqjh8</v>
@@ -1038,7 +1038,7 @@
         <v>Older adult, Male, No underlying conditions</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C19" s="5" t="str">
         <v>lbHoYiePn1V</v>
@@ -1060,7 +1060,7 @@
         <v>Older adult, Female</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C21" s="5" t="str">
         <v>Lwb0yEbt4s6</v>
@@ -1082,7 +1082,7 @@
         <v>Pfizer/Biontech/Comirnaty</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C23" s="5" t="str">
         <v>mpsnjgUuZA2</v>
@@ -1093,7 +1093,7 @@
         <v>Johnson&amp;Johnson</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C24" s="4" t="str">
         <v>mtgzsnM64tO</v>
@@ -1104,7 +1104,7 @@
         <v>Serious AEFI</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C25" s="5" t="str">
         <v>NyheW1iMbZ0</v>
@@ -1115,7 +1115,7 @@
         <v>AstraZeneca/AZD12222</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>2021-03-24</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C26" s="4" t="str">
         <v>p2wp5tC4iHi</v>
@@ -1126,7 +1126,7 @@
         <v>Gamaleya/Sputnik V</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C27" s="5" t="str">
         <v>paz8xJKpXiP</v>
@@ -1137,7 +1137,7 @@
         <v>AstraZeneca/AZ-SKBio</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C28" s="4" t="str">
         <v>Qa79VToX5lp</v>
@@ -1159,7 +1159,7 @@
         <v>AstraZeneca/AZD12222</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C30" s="4" t="str">
         <v>qxVEl8UH95p</v>
@@ -1170,7 +1170,7 @@
         <v>Moderna/mRNA-1273</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C31" s="5" t="str">
         <v>RBH7QWeF38A</v>
@@ -1192,7 +1192,7 @@
         <v>Sinopharm/Coronavac</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C33" s="5" t="str">
         <v>SHIcKoXyVDr</v>
@@ -1203,7 +1203,7 @@
         <v>Older adult, Female, Underlying conditions</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C34" s="4" t="str">
         <v>srFeKDklL1g</v>
@@ -1214,7 +1214,7 @@
         <v>Adult, Female, Underlying conditions</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C35" s="5" t="str">
         <v>Sw0WwH8AM10</v>
@@ -1225,7 +1225,7 @@
         <v>Gamaleya/Sputnik V</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C36" s="4" t="str">
         <v>TfnuN2akYGd</v>
@@ -1236,7 +1236,7 @@
         <v>Non-Serious AEFI</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C37" s="5" t="str">
         <v>uTh4A0HfrcV</v>
@@ -1258,7 +1258,7 @@
         <v>Older adult, Female, No underlying conditions</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C39" s="5" t="str">
         <v>UycnQgi3zDk</v>
@@ -1269,7 +1269,7 @@
         <v>Adult, Male</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C40" s="4" t="str">
         <v>VLskkRRCPef</v>
@@ -1280,7 +1280,7 @@
         <v>Sinopharm/Coronavac</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C41" s="5" t="str">
         <v>wikEP5C2Df2</v>
@@ -1313,7 +1313,7 @@
         <v>Vaccine2</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C44" s="4" t="str">
         <v>xIT1MPM7xSq</v>
@@ -1351,7 +1351,7 @@
         <v>Adults</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-04-21</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>Ch4XLC5v1hp</v>
@@ -1373,7 +1373,7 @@
         <v>COVIDVAC Vaccines(A)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>eMy3gCydKhI</v>
@@ -1418,7 +1418,7 @@
         <v>Pfizer/Biontech/Comirnaty(A)</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>BDSqsQYVrhJ</v>
@@ -1432,7 +1432,7 @@
         <v>AstraZeneca/AZ-SKBio(A)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>bPLfrCI6Jbb</v>
@@ -1474,7 +1474,7 @@
         <v>Moderna/mRNA-1273(A)</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>hcrDbPejaI6</v>
@@ -1488,7 +1488,7 @@
         <v>Adult</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2021-04-21</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>MyMzuzgT8IG</v>
@@ -1502,7 +1502,7 @@
         <v>Gamaleya/Sputnik V(A)</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>OkZnA874cN1</v>
@@ -1516,7 +1516,7 @@
         <v>Johnson&amp;Johnson(A)</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>TYz0ezPNNiz</v>
@@ -1530,7 +1530,7 @@
         <v>Older adult</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2021-04-21</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>u7WRRFCTdKU</v>
@@ -1544,7 +1544,7 @@
         <v>Sinopharm/Coronavac(A)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>vNV2D499eUM</v>
@@ -1558,7 +1558,7 @@
         <v>AstraZeneca/AZD12222(A)</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D12" s="4" t="str">
         <v>Z0LWdyopSII</v>
@@ -1735,7 +1735,7 @@
         <v>Opening balance + Received syringes</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G2" s="4" t="str">
         <v>AmlbDk8DLM5</v>
@@ -1758,7 +1758,7 @@
         <v>Opening balance + Received</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G3" s="5" t="str">
         <v>bmPhNsklLBs</v>
@@ -1781,7 +1781,7 @@
         <v>Opening balance + Received cold boxes</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G4" s="4" t="str">
         <v>BSpnHhts5Wq</v>
@@ -1804,7 +1804,7 @@
         <v>Opening balance + Received dilution syringes</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>fur5IpQTds0</v>
@@ -1827,7 +1827,7 @@
         <v>Opening balance + Received diluent</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>fvZTWJD32M8</v>
@@ -1850,7 +1850,7 @@
         <v>Opening balance + Received cold boxes</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>hoBv5eskXUz</v>
@@ -1873,7 +1873,7 @@
         <v>Discarded stock</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>jpln5wgIhws</v>
@@ -1896,7 +1896,7 @@
         <v>Opening balance + Received</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>jvlSrcKfSPy</v>
@@ -1919,7 +1919,7 @@
         <v>Opening balance + Received syringes with needle 1ml</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G10" s="4" t="str">
         <v>lEyHJSlCnN1</v>
@@ -1942,7 +1942,7 @@
         <v>Opening balance + Received vaccination cards</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G11" s="5" t="str">
         <v>oMGwL8PRVfR</v>
@@ -1965,7 +1965,7 @@
         <v>Opening balance + Received dilution syringes</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G12" s="4" t="str">
         <v>qfFxaurzC4l</v>
@@ -1988,7 +1988,7 @@
         <v>Opening balance + Received safety boxes</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G13" s="5" t="str">
         <v>RTgx10ZkMN1</v>
@@ -2011,7 +2011,7 @@
         <v>Opening balance + Received  safety boxes</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>T3K8J1BTIm4</v>
@@ -2034,7 +2034,7 @@
         <v>Opening balance + Received</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>vYrLYMDKavP</v>
@@ -2057,7 +2057,7 @@
         <v>Opening balance + Received</v>
       </c>
       <c r="F16" s="4" t="str">
-        <v>2021-04-21</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G16" s="4" t="str">
         <v>WoUY3PpG4rl</v>
@@ -2095,7 +2095,7 @@
         <v>COVIDVAC - Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-04-19</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>Z7DO3nEThHI</v>
@@ -2625,7 +2625,7 @@
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -2677,7 +2677,7 @@
         <v>Yes</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>AyprDvhGpNr</v>
@@ -2694,7 +2694,7 @@
         <v>Yes</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>gl7JRAdXkhR</v>
@@ -2711,7 +2711,7 @@
         <v>Yes</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>ZIajFXSOwEz</v>
@@ -2798,7 +2798,7 @@
         <v>Percentage</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J2" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -2830,7 +2830,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J3" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -2862,7 +2862,7 @@
         <v>Percentage</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J4" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -2894,7 +2894,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J5" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -2926,7 +2926,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J6" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -2958,7 +2958,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J7" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -2990,7 +2990,7 @@
         <v>Percentage</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J8" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3022,7 +3022,7 @@
         <v>Percentage</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J9" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3054,7 +3054,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J10" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3086,7 +3086,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J11" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3118,7 +3118,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J12" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3150,7 +3150,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J13" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3182,7 +3182,7 @@
         <v>Percentage</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J14" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3214,7 +3214,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J15" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3246,7 +3246,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I16" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J16" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3278,7 +3278,7 @@
         <v>Percentage</v>
       </c>
       <c r="I17" s="5" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J17" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3310,7 +3310,7 @@
         <v>Percentage</v>
       </c>
       <c r="I18" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J18" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3342,7 +3342,7 @@
         <v>Percentage</v>
       </c>
       <c r="I19" s="5" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J19" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3374,7 +3374,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I20" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J20" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3406,7 +3406,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I21" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J21" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3438,7 +3438,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I22" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J22" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3470,7 +3470,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I23" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J23" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3502,7 +3502,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I24" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J24" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3534,7 +3534,7 @@
         <v>Percentage</v>
       </c>
       <c r="I25" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J25" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3566,7 +3566,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I26" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J26" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3598,7 +3598,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I27" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J27" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3630,7 +3630,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I28" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J28" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3662,7 +3662,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I29" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J29" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3694,7 +3694,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I30" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J30" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3726,7 +3726,7 @@
         <v>Percentage</v>
       </c>
       <c r="I31" s="5" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J31" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3758,7 +3758,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I32" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J32" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3790,7 +3790,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I33" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J33" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3822,7 +3822,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I34" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J34" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3854,7 +3854,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I35" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J35" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3886,7 +3886,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I36" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J36" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3918,7 +3918,7 @@
         <v>Percentage</v>
       </c>
       <c r="I37" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J37" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3950,7 +3950,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I38" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J38" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3982,7 +3982,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I39" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J39" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4014,7 +4014,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I40" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J40" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4046,7 +4046,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I41" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J41" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4078,7 +4078,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I42" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J42" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4110,7 +4110,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I43" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J43" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4142,7 +4142,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I44" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J44" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4174,7 +4174,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I45" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J45" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4206,7 +4206,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I46" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J46" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4238,7 +4238,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I47" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J47" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4270,7 +4270,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I48" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J48" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4302,7 +4302,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I49" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J49" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4334,7 +4334,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I50" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J50" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4366,7 +4366,7 @@
         <v>Percentage</v>
       </c>
       <c r="I51" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J51" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4398,7 +4398,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I52" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J52" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4430,7 +4430,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I53" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J53" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4462,7 +4462,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I54" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J54" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4494,7 +4494,7 @@
         <v>Percentage</v>
       </c>
       <c r="I55" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J55" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4526,7 +4526,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I56" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J56" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4558,7 +4558,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I57" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J57" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4590,7 +4590,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I58" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J58" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4622,7 +4622,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I59" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J59" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4654,7 +4654,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I60" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J60" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4686,7 +4686,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I61" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J61" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4718,7 +4718,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I62" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J62" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4750,7 +4750,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I63" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J63" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4782,7 +4782,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I64" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J64" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4814,7 +4814,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I65" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J65" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4846,7 +4846,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I66" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J66" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4878,7 +4878,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I67" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J67" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4910,7 +4910,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I68" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J68" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4942,7 +4942,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I69" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J69" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -4974,7 +4974,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I70" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J70" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5006,7 +5006,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I71" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J71" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5038,7 +5038,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I72" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J72" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5070,7 +5070,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I73" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J73" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5102,7 +5102,7 @@
         <v>Percentage</v>
       </c>
       <c r="I74" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J74" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5134,7 +5134,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I75" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J75" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5166,7 +5166,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I76" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J76" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5198,7 +5198,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I77" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J77" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5230,7 +5230,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I78" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J78" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5262,7 +5262,7 @@
         <v>Percentage</v>
       </c>
       <c r="I79" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J79" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5294,7 +5294,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I80" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J80" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5326,7 +5326,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I81" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J81" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5358,7 +5358,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I82" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J82" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5390,7 +5390,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I83" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J83" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5422,7 +5422,7 @@
         <v>Percentage</v>
       </c>
       <c r="I84" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J84" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5454,7 +5454,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I85" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J85" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5486,7 +5486,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I86" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J86" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5518,7 +5518,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I87" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J87" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5550,7 +5550,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I88" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J88" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5582,7 +5582,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I89" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J89" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5614,7 +5614,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I90" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J90" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5646,7 +5646,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I91" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J91" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5678,7 +5678,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I92" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J92" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5710,7 +5710,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I93" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J93" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5742,7 +5742,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I94" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J94" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5774,7 +5774,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I95" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J95" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5806,7 +5806,7 @@
         <v>Percentage</v>
       </c>
       <c r="I96" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J96" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5838,7 +5838,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I97" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J97" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5870,7 +5870,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I98" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J98" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5902,7 +5902,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I99" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J99" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5934,7 +5934,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I100" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J100" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5966,7 +5966,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I101" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J101" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5998,7 +5998,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I102" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J102" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6030,7 +6030,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I103" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J103" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6062,7 +6062,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I104" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J104" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6094,7 +6094,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I105" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J105" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6126,7 +6126,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I106" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J106" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6158,7 +6158,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I107" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J107" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6190,7 +6190,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I108" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J108" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6222,7 +6222,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I109" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J109" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6254,7 +6254,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I110" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J110" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6286,7 +6286,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I111" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J111" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6318,7 +6318,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I112" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J112" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6350,7 +6350,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I113" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J113" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6382,7 +6382,7 @@
         <v>Percentage</v>
       </c>
       <c r="I114" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J114" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6414,7 +6414,7 @@
         <v>Percentage</v>
       </c>
       <c r="I115" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J115" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6446,7 +6446,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I116" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J116" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6478,7 +6478,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I117" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J117" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6510,7 +6510,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I118" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J118" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6542,7 +6542,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I119" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J119" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6574,7 +6574,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I120" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J120" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6606,7 +6606,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I121" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J121" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6638,7 +6638,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I122" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J122" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6670,7 +6670,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I123" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J123" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6702,7 +6702,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I124" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J124" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6734,7 +6734,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I125" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J125" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6766,7 +6766,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I126" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J126" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6798,7 +6798,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I127" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J127" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6830,7 +6830,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I128" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J128" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6862,7 +6862,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I129" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J129" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6894,7 +6894,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I130" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J130" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6926,7 +6926,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I131" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J131" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6958,7 +6958,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I132" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J132" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6990,7 +6990,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I133" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J133" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7022,7 +7022,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I134" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J134" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7054,7 +7054,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I135" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J135" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7086,7 +7086,7 @@
         <v>Percentage</v>
       </c>
       <c r="I136" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J136" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7118,7 +7118,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I137" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J137" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7150,7 +7150,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I138" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J138" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7182,7 +7182,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I139" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J139" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7214,7 +7214,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I140" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J140" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7246,7 +7246,7 @@
         <v>Percentage</v>
       </c>
       <c r="I141" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J141" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7278,7 +7278,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I142" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J142" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7310,7 +7310,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I143" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J143" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7342,7 +7342,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I144" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J144" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7374,7 +7374,7 @@
         <v>Percentage</v>
       </c>
       <c r="I145" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J145" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7406,7 +7406,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I146" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J146" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7438,7 +7438,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I147" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J147" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7470,7 +7470,7 @@
         <v>Percentage</v>
       </c>
       <c r="I148" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J148" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7502,7 +7502,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I149" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J149" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7534,7 +7534,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I150" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J150" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7566,7 +7566,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I151" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J151" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7598,7 +7598,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I152" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J152" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7630,7 +7630,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I153" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J153" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7662,7 +7662,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I154" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J154" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7694,7 +7694,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I155" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J155" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7726,7 +7726,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I156" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J156" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7758,7 +7758,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I157" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J157" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7790,7 +7790,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I158" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J158" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7822,7 +7822,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I159" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J159" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7854,7 +7854,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I160" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J160" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7886,7 +7886,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I161" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J161" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7918,7 +7918,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I162" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J162" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7950,7 +7950,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I163" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J163" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7982,7 +7982,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I164" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J164" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8014,7 +8014,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I165" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J165" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8046,7 +8046,7 @@
         <v>Percentage</v>
       </c>
       <c r="I166" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J166" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8078,7 +8078,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I167" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J167" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8110,7 +8110,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I168" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J168" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8142,7 +8142,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I169" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J169" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8174,7 +8174,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I170" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J170" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8206,7 +8206,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I171" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J171" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8238,7 +8238,7 @@
         <v>Percentage</v>
       </c>
       <c r="I172" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J172" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8270,7 +8270,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I173" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J173" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8302,7 +8302,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I174" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J174" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8334,7 +8334,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I175" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J175" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8366,7 +8366,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I176" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J176" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8398,7 +8398,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I177" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J177" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8430,7 +8430,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I178" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J178" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8462,7 +8462,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I179" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J179" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8494,7 +8494,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I180" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J180" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8526,7 +8526,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I181" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J181" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8558,7 +8558,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I182" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J182" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8590,7 +8590,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I183" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J183" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8622,7 +8622,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I184" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J184" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8654,7 +8654,7 @@
         <v>Percentage</v>
       </c>
       <c r="I185" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J185" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8686,7 +8686,7 @@
         <v>Percentage</v>
       </c>
       <c r="I186" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J186" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8718,7 +8718,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I187" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J187" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8750,7 +8750,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I188" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J188" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8782,7 +8782,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I189" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J189" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8814,7 +8814,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I190" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J190" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8846,7 +8846,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I191" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J191" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8878,7 +8878,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I192" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J192" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8910,7 +8910,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I193" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J193" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8942,7 +8942,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I194" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J194" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8974,7 +8974,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I195" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J195" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9006,7 +9006,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I196" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J196" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9038,7 +9038,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I197" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J197" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9070,7 +9070,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I198" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J198" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9102,7 +9102,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I199" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J199" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9134,7 +9134,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I200" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J200" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9166,7 +9166,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I201" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J201" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9198,7 +9198,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I202" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J202" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9230,7 +9230,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I203" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J203" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9262,7 +9262,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I204" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J204" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9294,7 +9294,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I205" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J205" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9326,7 +9326,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I206" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J206" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9358,7 +9358,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I207" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J207" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9390,7 +9390,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I208" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J208" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9422,7 +9422,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I209" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J209" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9454,7 +9454,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I210" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J210" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9486,7 +9486,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I211" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J211" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9518,7 +9518,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I212" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J212" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9550,7 +9550,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I213" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J213" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9582,7 +9582,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I214" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J214" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9614,7 +9614,7 @@
         <v>Percentage</v>
       </c>
       <c r="I215" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J215" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9646,7 +9646,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I216" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J216" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9678,7 +9678,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I217" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J217" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9710,7 +9710,7 @@
         <v>Percentage</v>
       </c>
       <c r="I218" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J218" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9742,7 +9742,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I219" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J219" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9774,7 +9774,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I220" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J220" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9806,7 +9806,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I221" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J221" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9838,7 +9838,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I222" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J222" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9870,7 +9870,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I223" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J223" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9902,7 +9902,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I224" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J224" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9934,7 +9934,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I225" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J225" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9966,7 +9966,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I226" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J226" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -9998,7 +9998,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I227" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J227" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10030,7 +10030,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I228" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J228" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10062,7 +10062,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I229" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J229" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10094,7 +10094,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I230" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J230" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10126,7 +10126,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I231" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J231" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10158,7 +10158,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I232" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J232" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10190,7 +10190,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I233" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J233" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10222,7 +10222,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I234" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J234" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10254,7 +10254,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I235" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J235" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10286,7 +10286,7 @@
         <v>Percentage</v>
       </c>
       <c r="I236" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J236" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10318,7 +10318,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I237" s="5" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J237" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10350,7 +10350,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I238" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J238" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10382,7 +10382,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I239" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J239" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10414,7 +10414,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I240" s="4" t="str">
-        <v>2021-04-15</v>
+        <v>2021-04-26</v>
       </c>
       <c r="J240" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -10511,7 +10511,7 @@
         <v>COVIDVAC - COVID-19 Vaccination Delivery</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>XAXoJuC3hvM</v>
@@ -11175,7 +11175,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>b8LigNTkhyG</v>
@@ -11189,7 +11189,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>B8tGSpVDYQR</v>
@@ -11203,7 +11203,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>CtbcfPoFCzo</v>
@@ -11217,7 +11217,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D5" s="5" t="str">
         <v>GYWAYluTnMj</v>
@@ -11231,7 +11231,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>H6lrQsOB7jA</v>
@@ -11245,7 +11245,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>hYDuLUBIdFj</v>
@@ -11259,7 +11259,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>KPQ6KeOZ9FX</v>
@@ -11273,7 +11273,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>KvXobGKUeNc</v>
@@ -11287,7 +11287,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>LWFnERgFj0F</v>
@@ -11301,7 +11301,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>ogY1C56Eiv9</v>
@@ -11315,7 +11315,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D12" s="4" t="str">
         <v>ouSGdU9G46U</v>
@@ -11329,7 +11329,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>PccWzAGw3o5</v>
@@ -11343,7 +11343,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D14" s="4" t="str">
         <v>r5oYja8d5jn</v>
@@ -11357,7 +11357,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D15" s="5" t="str">
         <v>TyijkItvgE3</v>
@@ -11371,7 +11371,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D16" s="4" t="str">
         <v>udHdm4Jtn7J</v>
@@ -11385,7 +11385,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D17" s="5" t="str">
         <v>wnbjrEvjqBs</v>
@@ -11430,7 +11430,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>D5EBdc7LDs6</v>
@@ -11444,7 +11444,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>ETiRgi3EXoS</v>
@@ -11458,7 +11458,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-04-21</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>FK69uGdqyM1</v>
@@ -11472,7 +11472,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D5" s="5" t="str">
         <v>hDix6ZMOB6p</v>
@@ -11486,7 +11486,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>K8F47kVnr77</v>
@@ -11500,7 +11500,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>MMEOBsXR6eE</v>
@@ -11514,7 +11514,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>NawHnMC4uVV</v>
@@ -11528,7 +11528,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>Q5AgE0cv3ou</v>
@@ -11542,7 +11542,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>TxHl78weq1n</v>
@@ -11556,7 +11556,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2021-04-16</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>YJDjqXkd0AF</v>
@@ -11601,7 +11601,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>mrhHfqYbv6m</v>
@@ -11615,7 +11615,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>nHhLZz3W50E</v>
@@ -11740,7 +11740,7 @@
         <v>COVAC admin</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>e2QMDWpq88P</v>
@@ -11751,7 +11751,7 @@
         <v>COVAC access</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2021-04-08</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>OeiDCnG3Pv2</v>
@@ -11834,7 +11834,7 @@
         <v>Doses per vaccine vial</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>rgWhPui0E7t</v>
@@ -11848,7 +11848,7 @@
         <v>Vaccine - stock status</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>Meln8vr9e8l</v>
@@ -11862,7 +11862,7 @@
         <v xml:space="preserve">Vaccine - stockout days </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>q4VeOYCNObp</v>
@@ -11876,7 +11876,7 @@
         <v>Other items - cold box</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D5" s="5" t="str">
         <v>tlfNOZiba1B</v>
@@ -11890,7 +11890,7 @@
         <v>Other items - diluent</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>O9DWoPLGDjv</v>
@@ -11904,7 +11904,7 @@
         <v>Other items - dilution syringes</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>O2chQ0pKrM1</v>
@@ -11918,7 +11918,7 @@
         <v>Other items - safety box</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>X1pWCgo7c7b</v>
@@ -11932,7 +11932,7 @@
         <v>Other items - syringes with needle 1ml</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>E6QwbBY6EER</v>
@@ -11946,7 +11946,7 @@
         <v>Other items - Vaccination cards</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>H83rr4eEQFJ</v>
@@ -11960,7 +11960,7 @@
         <v>Doses administered to front line health care workers (HCWs)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>wHEchl9ykRS</v>
@@ -11974,7 +11974,7 @@
         <v>Doses administered to essential workers</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D12" s="4" t="str">
         <v>QRw4oz7qRrK</v>
@@ -11988,7 +11988,7 @@
         <v>Doses administered to "Other" population</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>qYGHCtwfMzt</v>
@@ -12002,7 +12002,7 @@
         <v>Adverse Events Following Immunization</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D14" s="4" t="str">
         <v>gbLJpWp9sAH</v>
@@ -12016,7 +12016,7 @@
         <v>Vaccine wastage by reason</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D15" s="5" t="str">
         <v>UN4iEmCy6th</v>
@@ -12030,7 +12030,7 @@
         <v>Staff availability</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D16" s="4" t="str">
         <v>yH2LlrGMXzr</v>
@@ -12044,7 +12044,7 @@
         <v>Total population</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D17" s="5" t="str">
         <v>LxqibTCDI9U</v>
@@ -12058,7 +12058,7 @@
         <v>Total target populations</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D18" s="4" t="str">
         <v>MalimoojioF</v>
@@ -12072,7 +12072,7 @@
         <v>Disaggregated target populations</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D19" s="5" t="str">
         <v>I6FIWinQaAe</v>
@@ -12086,7 +12086,7 @@
         <v>People with underlying conditions</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D20" s="4" t="str">
         <v>rfCZkGgNApv</v>
@@ -13492,7 +13492,7 @@
         <v>Doses in a vial(Sinopharm/Coronavac)</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>cbRA6ZJJsmk</v>
@@ -13506,7 +13506,7 @@
         <v>Doses in a vial(AstraZeneca/AZD12222)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>Hazygnv9heS</v>
@@ -13520,7 +13520,7 @@
         <v>Doses in a vial(Moderna/mRNA-1273)</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>hEv6rCckL0w</v>
@@ -13534,7 +13534,7 @@
         <v>Doses in a vial(Pfizer/Biontech/Comirnaty)</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D5" s="5" t="str">
         <v>re4npNEWcDF</v>
@@ -13548,7 +13548,7 @@
         <v>Doses in a vial(Gamaleya/Sputnik V)</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2021-04-14</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>xxOEzzR2sVd</v>
@@ -13562,7 +13562,7 @@
         <v>Doses in a vial(Johnson&amp;Johnson)</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>xZpzitIJ3aU</v>
@@ -13576,7 +13576,7 @@
         <v>Doses in a vial(AstraZeneca/AZ-SKBio)</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>ylJ57nIwlYO</v>
@@ -13642,7 +13642,7 @@
         <v>default</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G2" s="4" t="str">
         <v>a6q0jTzVcip</v>
@@ -13665,7 +13665,7 @@
         <v>default</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G3" s="5" t="str">
         <v>ajqf0EsKxIC</v>
@@ -13688,7 +13688,7 @@
         <v>Adult/Sex</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G4" s="4" t="str">
         <v>arGTttrrqxE</v>
@@ -13711,7 +13711,7 @@
         <v>default</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>AxsGeK6Ug1O</v>
@@ -13734,7 +13734,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>bdsQugL5p5B</v>
@@ -13757,7 +13757,7 @@
         <v>default</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>bNPsOVqpBMj</v>
@@ -13780,7 +13780,7 @@
         <v>default</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>BYcRLORiKNG</v>
@@ -13803,7 +13803,7 @@
         <v>default</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>CctKBwpym8I</v>
@@ -13826,7 +13826,7 @@
         <v>default</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G10" s="4" t="str">
         <v>CTUdYPotCXF</v>
@@ -13849,7 +13849,7 @@
         <v>default</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G11" s="5" t="str">
         <v>dETqOgonm72</v>
@@ -13872,7 +13872,7 @@
         <v>default</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G12" s="4" t="str">
         <v>drljwLyAZQw</v>
@@ -13895,7 +13895,7 @@
         <v>default</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G13" s="5" t="str">
         <v>Dvx7RK4kXSI</v>
@@ -13918,7 +13918,7 @@
         <v>default</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>EgFl8yY2Te3</v>
@@ -13941,7 +13941,7 @@
         <v>default</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>EL8WnPd1ABT</v>
@@ -13964,7 +13964,7 @@
         <v>default</v>
       </c>
       <c r="F16" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G16" s="4" t="str">
         <v>emyAeGuGp8H</v>
@@ -13987,7 +13987,7 @@
         <v>default</v>
       </c>
       <c r="F17" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G17" s="5" t="str">
         <v>eoClH0iNeL4</v>
@@ -14010,7 +14010,7 @@
         <v>default</v>
       </c>
       <c r="F18" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G18" s="4" t="str">
         <v>eQX4WL751q0</v>
@@ -14033,7 +14033,7 @@
         <v>default</v>
       </c>
       <c r="F19" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G19" s="5" t="str">
         <v>F0Awi30X7xM</v>
@@ -14056,7 +14056,7 @@
         <v>default</v>
       </c>
       <c r="F20" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G20" s="4" t="str">
         <v>f0vfsLTNJzO</v>
@@ -14079,7 +14079,7 @@
         <v>default</v>
       </c>
       <c r="F21" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G21" s="5" t="str">
         <v>f3bOBccuyyo</v>
@@ -14102,7 +14102,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F22" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G22" s="4" t="str">
         <v>F7neHTcKur5</v>
@@ -14125,7 +14125,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="F23" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G23" s="5" t="str">
         <v>fjhkST9Cesq</v>
@@ -14148,7 +14148,7 @@
         <v>default</v>
       </c>
       <c r="F24" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G24" s="4" t="str">
         <v>foclaUCiq6S</v>
@@ -14171,7 +14171,7 @@
         <v>AEFI Severity</v>
       </c>
       <c r="F25" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G25" s="5" t="str">
         <v>Gpnjeds5dkE</v>
@@ -14194,7 +14194,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="F26" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G26" s="4" t="str">
         <v>H4jwFdAA1fm</v>
@@ -14217,7 +14217,7 @@
         <v>default</v>
       </c>
       <c r="F27" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G27" s="5" t="str">
         <v>hmlw3sNoOI1</v>
@@ -14240,7 +14240,7 @@
         <v>default</v>
       </c>
       <c r="F28" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G28" s="4" t="str">
         <v>hPCE24XXDAW</v>
@@ -14263,7 +14263,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F29" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G29" s="5" t="str">
         <v>iP4hjDgtgPq</v>
@@ -14286,7 +14286,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="F30" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G30" s="4" t="str">
         <v>JRMAR84ICCG</v>
@@ -14309,7 +14309,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="F31" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G31" s="5" t="str">
         <v>kevh9LGj0mX</v>
@@ -14332,7 +14332,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="F32" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G32" s="4" t="str">
         <v>KG6W0tUl8O3</v>
@@ -14355,7 +14355,7 @@
         <v>default</v>
       </c>
       <c r="F33" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G33" s="5" t="str">
         <v>kl0xOGWS6ww</v>
@@ -14378,7 +14378,7 @@
         <v>default</v>
       </c>
       <c r="F34" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G34" s="4" t="str">
         <v>KnFWsoy4UYs</v>
@@ -14401,7 +14401,7 @@
         <v>default</v>
       </c>
       <c r="F35" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G35" s="5" t="str">
         <v>KrAF26CuNrx</v>
@@ -14424,7 +14424,7 @@
         <v>default</v>
       </c>
       <c r="F36" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G36" s="4" t="str">
         <v>kyYlvg9iV6e</v>
@@ -14447,7 +14447,7 @@
         <v>default</v>
       </c>
       <c r="F37" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G37" s="5" t="str">
         <v>l19W7jOdEu2</v>
@@ -14470,7 +14470,7 @@
         <v>default</v>
       </c>
       <c r="F38" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G38" s="4" t="str">
         <v>mmcdLpzPJ8C</v>
@@ -14493,7 +14493,7 @@
         <v>default</v>
       </c>
       <c r="F39" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G39" s="5" t="str">
         <v>Nm8VHHFGIyY</v>
@@ -14516,7 +14516,7 @@
         <v>default</v>
       </c>
       <c r="F40" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G40" s="4" t="str">
         <v>NrXl6iNxtWb</v>
@@ -14539,7 +14539,7 @@
         <v>default</v>
       </c>
       <c r="F41" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G41" s="5" t="str">
         <v>O8FZejiaZEk</v>
@@ -14562,7 +14562,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F42" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G42" s="4" t="str">
         <v>oG5V31NvLZO</v>
@@ -14585,7 +14585,7 @@
         <v>default</v>
       </c>
       <c r="F43" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G43" s="5" t="str">
         <v>oh6IWG1wYA3</v>
@@ -14608,7 +14608,7 @@
         <v>default</v>
       </c>
       <c r="F44" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G44" s="4" t="str">
         <v>oS6wBIaveFo</v>
@@ -14631,7 +14631,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F45" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G45" s="5" t="str">
         <v>ovTS34BBoUi</v>
@@ -14654,7 +14654,7 @@
         <v>default</v>
       </c>
       <c r="F46" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G46" s="4" t="str">
         <v>pkXVIqIHHVa</v>
@@ -14677,7 +14677,7 @@
         <v>default</v>
       </c>
       <c r="F47" s="5" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G47" s="5" t="str">
         <v>ppcgPRAW9b9</v>
@@ -14700,7 +14700,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="F48" s="4" t="str">
-        <v>2021-04-22</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G48" s="4" t="str">
         <v>pr5KCf5nkrZ</v>
@@ -14723,7 +14723,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F49" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G49" s="5" t="str">
         <v>pVrVmrRU0cz</v>
@@ -14746,7 +14746,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="F50" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G50" s="4" t="str">
         <v>qQBypsWpkwZ</v>
@@ -14769,7 +14769,7 @@
         <v>default</v>
       </c>
       <c r="F51" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G51" s="5" t="str">
         <v>QWaRooSTLPr</v>
@@ -14792,7 +14792,7 @@
         <v>default</v>
       </c>
       <c r="F52" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G52" s="4" t="str">
         <v>RLraPla6D9Q</v>
@@ -14815,7 +14815,7 @@
         <v>default</v>
       </c>
       <c r="F53" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G53" s="5" t="str">
         <v>S2lAb8nKCHb</v>
@@ -14838,7 +14838,7 @@
         <v>default</v>
       </c>
       <c r="F54" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G54" s="4" t="str">
         <v>SaHOUWuc0aL</v>
@@ -14861,7 +14861,7 @@
         <v>default</v>
       </c>
       <c r="F55" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G55" s="5" t="str">
         <v>scDzaP4Qf7n</v>
@@ -14884,7 +14884,7 @@
         <v>default</v>
       </c>
       <c r="F56" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G56" s="4" t="str">
         <v>segUqhr3Bmn</v>
@@ -14907,7 +14907,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F57" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G57" s="5" t="str">
         <v>Snc1asgJ7sT</v>
@@ -14930,7 +14930,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F58" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G58" s="4" t="str">
         <v>T5yXrDEuwzL</v>
@@ -14953,7 +14953,7 @@
         <v>default</v>
       </c>
       <c r="F59" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G59" s="5" t="str">
         <v>tg60B4x2trg</v>
@@ -14976,7 +14976,7 @@
         <v>Vial condition/Wastage reasons</v>
       </c>
       <c r="F60" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G60" s="4" t="str">
         <v>TINjydYZyb0</v>
@@ -14999,7 +14999,7 @@
         <v>default</v>
       </c>
       <c r="F61" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G61" s="5" t="str">
         <v>tmHKRG9itcO</v>
@@ -15022,7 +15022,7 @@
         <v>default</v>
       </c>
       <c r="F62" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G62" s="4" t="str">
         <v>tnpNBvvniAM</v>
@@ -15045,7 +15045,7 @@
         <v>default</v>
       </c>
       <c r="F63" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G63" s="5" t="str">
         <v>u0tQHrxtfVP</v>
@@ -15068,7 +15068,7 @@
         <v>default</v>
       </c>
       <c r="F64" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G64" s="4" t="str">
         <v>u90k7rEUGX0</v>
@@ -15091,7 +15091,7 @@
         <v>default</v>
       </c>
       <c r="F65" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G65" s="5" t="str">
         <v>vdHrKoTsyAe</v>
@@ -15114,7 +15114,7 @@
         <v>default</v>
       </c>
       <c r="F66" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G66" s="4" t="str">
         <v>vnhYE8Muoj8</v>
@@ -15137,7 +15137,7 @@
         <v>default</v>
       </c>
       <c r="F67" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G67" s="5" t="str">
         <v>WAQp0YiVml3</v>
@@ -15160,7 +15160,7 @@
         <v>default</v>
       </c>
       <c r="F68" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G68" s="4" t="str">
         <v>WCqFMZu8xby</v>
@@ -15183,7 +15183,7 @@
         <v>default</v>
       </c>
       <c r="F69" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G69" s="5" t="str">
         <v>wLLWlLFKJTL</v>
@@ -15206,7 +15206,7 @@
         <v>default</v>
       </c>
       <c r="F70" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G70" s="4" t="str">
         <v>x7my3g8Fvaz</v>
@@ -15229,7 +15229,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="F71" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G71" s="5" t="str">
         <v>xcvzLIJcUwm</v>
@@ -15252,7 +15252,7 @@
         <v>default</v>
       </c>
       <c r="F72" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G72" s="4" t="str">
         <v>XSzYgW92sBI</v>
@@ -15275,7 +15275,7 @@
         <v>default</v>
       </c>
       <c r="F73" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G73" s="5" t="str">
         <v>y4Bs6d0hNoL</v>
@@ -15298,7 +15298,7 @@
         <v>Adult/Sex</v>
       </c>
       <c r="F74" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G74" s="4" t="str">
         <v>yBXYpUZwZS6</v>
@@ -15321,7 +15321,7 @@
         <v>Adult/Sex</v>
       </c>
       <c r="F75" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G75" s="5" t="str">
         <v>YtJqjif8Gne</v>
@@ -15344,7 +15344,7 @@
         <v>default</v>
       </c>
       <c r="F76" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G76" s="4" t="str">
         <v>zeFAEBgGrEx</v>
@@ -15367,7 +15367,7 @@
         <v>default</v>
       </c>
       <c r="F77" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G77" s="5" t="str">
         <v>zqptPF1iBGE</v>
@@ -15390,7 +15390,7 @@
         <v>Adult/Sex</v>
       </c>
       <c r="F78" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G78" s="4" t="str">
         <v>zsbo4sda5sT</v>
@@ -15413,7 +15413,7 @@
         <v>default</v>
       </c>
       <c r="F79" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="G79" s="5" t="str">
         <v>ZuNdVpukYld</v>
@@ -16102,7 +16102,7 @@
         <v>Adult/Sex</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>AJ2NILzEPpt</v>
@@ -16130,7 +16130,7 @@
         <v>COVIDVAC Vaccines (attrib)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>iPEQ4nCZD29</v>
@@ -16144,7 +16144,7 @@
         <v>Adults/Sex/Conditions</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2021-04-13</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>OqByN3juZca</v>
@@ -16158,7 +16158,7 @@
         <v>Vial condition/Wastage reasons</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-02-24</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>P9CXpIYGFBR</v>
@@ -16172,7 +16172,7 @@
         <v>COVIDVAC Vaccines (disagg)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2021-04-17</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>wiB5JPPk2vC</v>
@@ -16186,7 +16186,7 @@
         <v>AEFI Severity</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2021-03-25</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>XRwDg6XbP10</v>
@@ -16245,7 +16245,7 @@
         <v>COVIDVAC Vaccines (D)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>EFELXPfSph0</v>
@@ -16315,7 +16315,7 @@
         <v>Underlying conditions YN</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2021-03-24</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>tbz69LPobVY</v>
@@ -16329,7 +16329,7 @@
         <v>Adults</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2021-04-21</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C9" s="5" t="str">
         <v>TY1ViLCm2II</v>
@@ -16343,7 +16343,7 @@
         <v>COVIDVAC Vaccines (A)</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-04-26</v>
       </c>
       <c r="C10" s="4" t="str">
         <v>XN3meiBvJlX</v>

</xml_diff>

<commit_message>
feat: Update COVIDVAC for D2v 2.30, 2.33, 2.34, 2.35
</commit_message>
<xml_diff>
--- a/metadata/COVIDVAC/COVIDVAC_COMPLETE_V1_DHIS2.30/reference.xlsx
+++ b/metadata/COVIDVAC/COVIDVAC_COMPLETE_V1_DHIS2.30/reference.xlsx
@@ -441,13 +441,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -471,7 +471,7 @@
         <v>Type</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COMPLETE</v>
+        <v>AGGREGATE</v>
       </c>
     </row>
     <row r="4">
@@ -479,7 +479,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>V1.2</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5">
@@ -487,23 +487,31 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.30</v>
+        <v>2.30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Created</v>
+        <v>DHIS2 build</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-04-26T16:17</v>
+        <v>6af6fc0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Identifier</v>
+        <v>Last updated</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVIDVAC_COMPLETE_V1.2_DHIS2.30_2021-04-26T16:17</v>
+        <v>20210915T084638</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v>COVIDVAC_AGGREGATE_V1.2_2.30-en</v>
       </c>
     </row>
   </sheetData>
@@ -2677,7 +2685,7 @@
         <v>Yes</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>2021-04-26</v>
+        <v>2021-06-17</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>AyprDvhGpNr</v>
@@ -2711,7 +2719,7 @@
         <v>Yes</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-28</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>ZIajFXSOwEz</v>
@@ -3307,10 +3315,10 @@
         <v>1</v>
       </c>
       <c r="H18" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I18" s="4" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J18" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -3918,7 +3926,7 @@
         <v>Percentage</v>
       </c>
       <c r="I37" s="5" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J37" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5198,7 +5206,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I77" s="5" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J77" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -5422,7 +5430,7 @@
         <v>Percentage</v>
       </c>
       <c r="I84" s="4" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J84" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -6414,7 +6422,7 @@
         <v>Percentage</v>
       </c>
       <c r="I115" s="5" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J115" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -7086,7 +7094,7 @@
         <v>Percentage</v>
       </c>
       <c r="I136" s="4" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J136" s="4" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8654,7 +8662,7 @@
         <v>Percentage</v>
       </c>
       <c r="I185" s="5" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J185" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -8782,7 +8790,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I189" s="5" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-29</v>
       </c>
       <c r="J189" s="5" t="str">
         <v>TIIiQ09g7Bl</v>
@@ -11714,12 +11722,12 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -11737,23 +11745,34 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVAC admin</v>
+        <v>COVAC data capture</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-04-26</v>
+        <v>2021-09-15</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>e2QMDWpq88P</v>
+        <v>AxmuDEHQApq</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
+        <v>COVAC admin</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>2021-04-26</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>e2QMDWpq88P</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
         <v>COVAC access</v>
       </c>
-      <c r="B3" s="5" t="str">
-        <v>2021-04-26</v>
-      </c>
-      <c r="C3" s="5" t="str">
+      <c r="B4" s="4" t="str">
+        <v>2021-04-26</v>
+      </c>
+      <c r="C4" s="4" t="str">
         <v>OeiDCnG3Pv2</v>
       </c>
     </row>
@@ -11801,7 +11820,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -12058,7 +12077,7 @@
         <v>Total target populations</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-28</v>
       </c>
       <c r="D18" s="4" t="str">
         <v>MalimoojioF</v>
@@ -12072,24 +12091,10 @@
         <v>Disaggregated target populations</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>2021-04-26</v>
+        <v>2021-04-28</v>
       </c>
       <c r="D19" s="5" t="str">
         <v>I6FIWinQaAe</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>COVIDVAC - Population (Yearly)</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>People with underlying conditions</v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <v>2021-04-26</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <v>rfCZkGgNApv</v>
       </c>
     </row>
   </sheetData>
@@ -13302,7 +13307,7 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B71" s="5" t="str">
         <v>Total population</v>
@@ -13319,7 +13324,7 @@
     </row>
     <row r="72">
       <c r="A72" s="4" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B72" s="4" t="str">
         <v>Total target populations</v>
@@ -13336,7 +13341,7 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B73" s="5" t="str">
         <v>Total target populations</v>
@@ -13353,7 +13358,7 @@
     </row>
     <row r="74">
       <c r="A74" s="4" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B74" s="4" t="str">
         <v>Total target populations</v>
@@ -13362,32 +13367,32 @@
         <v>MalimoojioF</v>
       </c>
       <c r="D74" s="4" t="str">
-        <v>COVIDVAC - Total Other population</v>
+        <v>COVIDVAC - Total people with at least one underlying condition</v>
       </c>
       <c r="E74" s="4" t="str">
-        <v>emyAeGuGp8H</v>
+        <v>mmcdLpzPJ8C</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B75" s="5" t="str">
-        <v>Disaggregated target populations</v>
+        <v>Total target populations</v>
       </c>
       <c r="C75" s="5" t="str">
-        <v>I6FIWinQaAe</v>
+        <v>MalimoojioF</v>
       </c>
       <c r="D75" s="5" t="str">
-        <v>COVIDVAC - Target frontline healthcare workers</v>
+        <v>COVIDVAC - Total Other population</v>
       </c>
       <c r="E75" s="5" t="str">
-        <v>zsbo4sda5sT</v>
+        <v>emyAeGuGp8H</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="4" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B76" s="4" t="str">
         <v>Disaggregated target populations</v>
@@ -13396,15 +13401,15 @@
         <v>I6FIWinQaAe</v>
       </c>
       <c r="D76" s="4" t="str">
-        <v>COVIDVAC - Target essential workers</v>
+        <v>COVIDVAC - Target frontline healthcare workers</v>
       </c>
       <c r="E76" s="4" t="str">
-        <v>yBXYpUZwZS6</v>
+        <v>zsbo4sda5sT</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="5" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B77" s="5" t="str">
         <v>Disaggregated target populations</v>
@@ -13413,44 +13418,44 @@
         <v>I6FIWinQaAe</v>
       </c>
       <c r="D77" s="5" t="str">
-        <v>COVIDVAC - Target other population</v>
+        <v>COVIDVAC - Target essential workers</v>
       </c>
       <c r="E77" s="5" t="str">
-        <v>arGTttrrqxE</v>
+        <v>yBXYpUZwZS6</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="4" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B78" s="4" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="C78" s="4" t="str">
-        <v>rfCZkGgNApv</v>
+        <v>I6FIWinQaAe</v>
       </c>
       <c r="D78" s="4" t="str">
-        <v>COVIDVAC - Total people with at least one underlying condition</v>
+        <v>COVIDVAC - Target people with at least one underlying condition</v>
       </c>
       <c r="E78" s="4" t="str">
-        <v>mmcdLpzPJ8C</v>
+        <v>YtJqjif8Gne</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="5" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="B79" s="5" t="str">
-        <v>People with underlying conditions</v>
+        <v>Disaggregated target populations</v>
       </c>
       <c r="C79" s="5" t="str">
-        <v>rfCZkGgNApv</v>
+        <v>I6FIWinQaAe</v>
       </c>
       <c r="D79" s="5" t="str">
-        <v>COVIDVAC - Target people with at least one underlying condition</v>
+        <v>COVIDVAC - Target other population</v>
       </c>
       <c r="E79" s="5" t="str">
-        <v>YtJqjif8Gne</v>
+        <v>arGTttrrqxE</v>
       </c>
     </row>
   </sheetData>
@@ -16287,7 +16292,7 @@
         <v>default</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-04-20</v>
+        <v>2021-09-13</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>GLevLNI9wkl</v>

</xml_diff>